<commit_message>
revisi 25 april 2025
</commit_message>
<xml_diff>
--- a/Post/Index/data/Result - Machine learning Evaluation.xlsx
+++ b/Post/Index/data/Result - Machine learning Evaluation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,32 +436,17 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>train mae</t>
+          <t>mae</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>train mape</t>
+          <t>mape</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>train rmse</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>test mae</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>test mape</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>test rmse</t>
+          <t>rmse</t>
         </is>
       </c>
     </row>
@@ -472,22 +457,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.340961639895411</v>
+        <v>1.23</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05047347821172429</v>
+        <v>0.04</v>
       </c>
       <c r="D2" t="n">
-        <v>1.720161566315168</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.8077697826826057</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.02867362888555341</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1.064016659330977</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="3">
@@ -497,22 +473,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7.593125226826011</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0819002490117183</v>
+        <v>0.06</v>
       </c>
       <c r="D3" t="n">
-        <v>11.80141865722994</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2.828887416903832</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.03001426346560658</v>
-      </c>
-      <c r="G3" t="n">
-        <v>6.163670531791811</v>
+        <v>7.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revisi 30 april 2025
</commit_message>
<xml_diff>
--- a/Post/Index/data/Result - Machine learning Evaluation.xlsx
+++ b/Post/Index/data/Result - Machine learning Evaluation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,50 +436,83 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>mae</t>
+          <t>train_mae</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>mape</t>
+          <t>train_mape</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>rmse</t>
+          <t>train_rmse</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>test_mae</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>test_mape</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>test_rmse</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Suhu Udara</t>
+          <t>Suhu Udara (°C)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.23</v>
+        <v>1.28</v>
       </c>
       <c r="C2" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="D2" t="n">
-        <v>1.7</v>
+        <v>1.67</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1.03</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Kelembapan</t>
+          <t>Kelembapan (%)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6.84</v>
       </c>
       <c r="C3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D3" t="n">
-        <v>7.1</v>
+        <v>9.99</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>